<commit_message>
Report and figure update
Figures and Report text for analyses with DepMap cell lines
</commit_message>
<xml_diff>
--- a/report/tables.xlsx
+++ b/report/tables.xlsx
@@ -79790,7 +79790,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -79819,6 +79819,11 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>DepMap cell lines</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>HPA</t>
         </is>
       </c>
@@ -79846,6 +79851,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>80</t>
         </is>
       </c>
@@ -79873,6 +79883,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>log₂ gene count</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>IHC score</t>
         </is>
       </c>
@@ -79902,6 +79917,12 @@
         </is>
       </c>
       <c r="E4" t="inlineStr">
+        <is>
+          <t>3.2 [IQR: 1.8 - 5]
+range: 0.07 - 8.2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>6 [IQR: 4 - 9]
 range: 1 - 12
@@ -79935,6 +79956,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>3.2 [IQR: 1.2 - 4]
+range: 0.029 - 6.3</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>1.5 [IQR: 1 - 6]
 range: 1 - 9
 complete: n = 18</t>
@@ -79967,6 +79994,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>1.9 [IQR: 0.65 - 4.7]
+range: 0.18 - 8.2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>6 [IQR: 1 - 8.5]
 range: 1 - 16
 complete: n = 11</t>
@@ -79999,6 +80032,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>1.4 [IQR: 0.57 - 2.4]
+range: 0.12 - 5.3</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>6 [IQR: 4 - 8]
 range: 2 - 12
 complete: n = 18</t>
@@ -80031,6 +80070,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>4.1 [IQR: 3.1 - 4.7]
+range: 1.8 - 5.7</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>6 [IQR: 5.5 - 8]
 range: 1 - 8
 complete: n = 12</t>
@@ -80063,6 +80108,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>1.8 [IQR: 1.1 - 3.2]
+range: 0.12 - 5.6</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>2 [IQR: 1 - 4]
 range: 1 - 12
 complete: n = 16</t>
@@ -80095,6 +80146,12 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>0.29 [IQR: 0.07 - 1.1]
+range: 0 - 3.8</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>1 [IQR: 1 - 1]
 range: 1 - 1
 complete: n = 11</t>
@@ -80127,6 +80184,12 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>1.3 [IQR: 0.098 - 4.1]
+range: 0 - 5.3</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>1 [IQR: 1 - 1]
 range: 1 - 6
 complete: n = 23</t>
@@ -80153,6 +80216,12 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 0.58</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>4 [IQR: 1 - 6]
 range: 1 - 6
 complete: n = 12</t>
@@ -80179,6 +80248,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 0.014</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>1 [IQR: 1 - 1]
 range: 1 - 4
 complete: n = 11</t>
@@ -80209,6 +80284,12 @@
 range: -2.3 - 0.79</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0.38 [IQR: 0.029 - 1.9]
+range: 0 - 6.2</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -80228,6 +80309,12 @@
 range: 0 - 2.3</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 0</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -80254,6 +80341,12 @@
         </is>
       </c>
       <c r="E16" t="inlineStr">
+        <is>
+          <t>0.029 [IQR: 0 - 0.098]
+range: 0 - 6.3</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
         <is>
           <t>2.5 [IQR: 1 - 6.5]
 range: 1 - 12
@@ -80279,6 +80372,12 @@
 range: 0 - 4.9</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.12]
+range: 0 - 0.75</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -80305,6 +80404,12 @@
         </is>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>0.043 [IQR: 0 - 0.098]
+range: 0 - 0.63</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
         <is>
           <t>1 [IQR: 1 - 1]
 range: 1 - 6
@@ -80338,6 +80443,12 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 0.4</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
           <t>6 [IQR: 6 - 6.5]
 range: 6 - 8
 complete: n = 12</t>
@@ -80370,6 +80481,12 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>1.7 [IQR: 1.2 - 3]
+range: 0.07 - 5.1</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>1 [IQR: 1 - 1]
 range: 1 - 1
 complete: n = 11</t>
@@ -80400,6 +80517,12 @@
 range: -2.1 - 0.6</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0.69 [IQR: 0.28 - 1.7]
+range: 0 - 3.6</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -80425,6 +80548,12 @@
 range: -1.8 - 0.73</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.21 [IQR: 0.07 - 1.5]
+range: 0 - 5.4</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -80450,6 +80579,12 @@
 range: -1.5 - 0.89</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0.07 [IQR: 0.014 - 0.43]
+range: 0 - 1.2</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -80476,6 +80611,12 @@
         </is>
       </c>
       <c r="E24" t="inlineStr">
+        <is>
+          <t>0.07 [IQR: 0 - 0.18]
+range: 0 - 0.6</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
         <is>
           <t>1 [IQR: 1 - 4.5]
 range: 1 - 9
@@ -80509,6 +80650,12 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
+          <t>0.11 [IQR: 0.043 - 0.25]
+range: 0 - 1.2</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
           <t>1 [IQR: 1 - 1]
 range: 1 - 6
 complete: n = 11</t>
@@ -80535,6 +80682,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
+          <t>0.043 [IQR: 0 - 0.23]
+range: 0 - 4.7</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
           <t>4 [IQR: 1 - 6]
 range: 1 - 12
 complete: n = 12</t>
@@ -80559,6 +80712,12 @@
 range: 0 - 6.5</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.029]
+range: 0 - 0.53</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -80579,6 +80738,12 @@
         </is>
       </c>
       <c r="E28" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.057]
+range: 0 - 1.8</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
         <is>
           <t>1 [IQR: 1 - 1]
 range: 1 - 1
@@ -80610,6 +80775,12 @@
 range: -2.3 - 0.0028</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>0.15 [IQR: 0.029 - 0.23]
+range: 0 - 0.61</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -80635,6 +80806,12 @@
 range: -2.4 - 0.028</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0]
+range: 0 - 0.029</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -80661,6 +80838,12 @@
         </is>
       </c>
       <c r="E31" t="inlineStr">
+        <is>
+          <t>3.3 [IQR: 0.98 - 6.5]
+range: 0.11 - 9.4</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
         <is>
           <t>1 [IQR: 1 - 8]
 range: 1 - 12
@@ -80692,6 +80875,12 @@
 range: -2.3 - 0.84</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>0 [IQR: 0 - 0.043]
+range: 0 - 0.3</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -80718,6 +80907,12 @@
         </is>
       </c>
       <c r="E33" t="inlineStr">
+        <is>
+          <t>0.82 [IQR: 0.59 - 1.1]
+range: 0.25 - 2.4</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
         <is>
           <t>1 [IQR: 1 - 1]
 range: 1 - 1
@@ -80749,6 +80944,12 @@
 range: -1.7 - 1.4</t>
         </is>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0.014 [IQR: 0 - 0.43]
+range: 0 - 5.4</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -80775,6 +80976,12 @@
         </is>
       </c>
       <c r="E35" t="inlineStr">
+        <is>
+          <t>0.084 [IQR: 0.029 - 0.2]
+range: 0 - 5.1</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
         <is>
           <t>8 [IQR: 5.5 - 8]
 range: 1 - 12
@@ -80808,6 +81015,12 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
+          <t>2.1 [IQR: 0.59 - 4.3]
+range: 0.014 - 8.6</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
           <t>6 [IQR: 2.5 - 7]
 range: 1 - 12
 complete: n = 11</t>
@@ -80840,6 +81053,12 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
+          <t>6.6 [IQR: 5.7 - 7.5]
+range: 4.1 - 8.4</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
           <t>8 [IQR: 1 - 12]
 range: 1 - 16
 complete: n = 32</t>
@@ -80872,6 +81091,12 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
+          <t>1.2 [IQR: 0.45 - 2.7]
+range: 0 - 7.1</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
           <t>12 [IQR: 12 - 14]
 range: 4 - 16
 complete: n = 11</t>
@@ -80904,6 +81129,12 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
+          <t>7.2 [IQR: 6.9 - 7.8]
+range: 4.5 - 8.2</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
           <t>9 [IQR: 6.5 - 11]
 range: 4 - 16
 complete: n = 14</t>
@@ -80936,6 +81167,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
+          <t>0.42 [IQR: 0.084 - 0.89]
+range: 0 - 7.2</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
           <t>2 [IQR: 1 - 8.2]
 range: 1 - 16
 complete: n = 30</t>
@@ -80968,6 +81205,12 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
+          <t>8 [IQR: 7.3 - 8.6]
+range: 0.41 - 9.9</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
           <t>5 [IQR: 1.2 - 12]
 range: 1 - 16
 complete: n = 26</t>
@@ -81000,6 +81243,12 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
+          <t>5 [IQR: 4 - 5.9]
+range: 1.3 - 8</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
           <t>2 [IQR: 1 - 8]
 range: 1 - 12
 complete: n = 25</t>
@@ -81030,6 +81279,12 @@
 range: 0.079 - 1.7</t>
         </is>
       </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>5.6 [IQR: 5.1 - 6.4]
+range: 3.7 - 7.6</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -81055,6 +81310,12 @@
 range: -2.4 - 0.78</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0.39 [IQR: 0.07 - 0.96]
+range: 0 - 5.1</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -81081,6 +81342,12 @@
         </is>
       </c>
       <c r="E45" t="inlineStr">
+        <is>
+          <t>2.4 [IQR: 0.19 - 3.7]
+range: 0 - 5.6</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
         <is>
           <t>8 [IQR: 4.8 - 12]
 range: 1 - 16
@@ -81114,6 +81381,12 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
+          <t>0.07 [IQR: 0 - 0.12]
+range: 0 - 5.8</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
           <t>1 [IQR: 1 - 5]
 range: 1 - 12
 complete: n = 19</t>
@@ -81146,6 +81419,12 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
+          <t>6.1 [IQR: 5.9 - 6.4]
+range: 4.4 - 7.4</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
           <t>1 [IQR: 1 - 4]
 range: 1 - 8
 complete: n = 11</t>
@@ -81174,6 +81453,12 @@
         <is>
           <t>-0.0079 [IQR: -0.32 - 0.22]
 range: -1.2 - 1.2</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>0.93 [IQR: 0.084 - 2.6]
+range: 0 - 5.5</t>
         </is>
       </c>
     </row>

</xml_diff>